<commit_message>
updated with changes made
</commit_message>
<xml_diff>
--- a/data/ALLOptions.xlsx
+++ b/data/ALLOptions.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8689887-5225-464C-986E-3DEEF87ECE66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,6 +340,13 @@
 Some images within this record are not available because they contain medically sensitive information.</t>
   </si>
   <si>
+    <t>Ordering and viewing options
+Free
+Download size approximately 1 MB. Download format PDF
+Add to basket
+More ways to view this record</t>
+  </si>
+  <si>
     <t>http://test.discovery.nationalarchives.gov.uk/details/r/C5687975?readertype=staffin</t>
   </si>
   <si>
@@ -406,9 +414,6 @@
   </si>
   <si>
     <t>http://test.discovery.nationalarchives.gov.uk/details/c/F133246?readertype=staffin</t>
-  </si>
-  <si>
-    <t>http://test.discovery.nationalarchives.gov.uk/details/r/C543337?readertype=staffin</t>
   </si>
   <si>
     <t>http://test.discovery.nationalarchives.gov.uk/details/r/90ad00a1aa6149efa3991fab6037a5ec?readertype=staffin</t>
@@ -426,6 +431,12 @@
     <t>How to view this record:
 Request a quote for a copy to be sent to you via email or post (£)
 Order a copy
+More ways to view this record</t>
+  </si>
+  <si>
+    <t>Download this record
+Download size approximately 1 MB. Download format PDF
+Download now
 More ways to view this record</t>
   </si>
   <si>
@@ -472,23 +483,13 @@
 To request a search of closed records you are required to upload documents as proof that the person is no longer living. However, for security reasons, the computer terminals in our reading rooms do not allow documents to be uploaded. To request a search of closed records please access our website from outside The National Archives.</t>
   </si>
   <si>
-    <t>Download this record
-Download size approximately 1.5 MB. Download format PDF
-Download now
-More ways to view this record</t>
-  </si>
-  <si>
-    <t>Ordering and viewing options
-Free
-Download size approximately 1.5 MB. Download format PDF
-Add to basket
-More ways to view this record</t>
+    <t>https://test.discovery.nationalarchives.gov.uk/details/r/C198022?readertype=staffin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,6 +547,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -593,7 +597,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,9 +630,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,6 +682,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -836,11 +874,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +897,7 @@
     <col min="12" max="12" width="33.28515625" style="1" customWidth="1"/>
     <col min="13" max="13" width="43.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="35.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="31.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
     <col min="16" max="16" width="39.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="24" style="1" customWidth="1"/>
     <col min="18" max="18" width="19.28515625" style="1" customWidth="1"/>
@@ -980,97 +1018,97 @@
     </row>
     <row r="2" spans="1:32" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>98</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>99</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>100</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>101</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>98</v>
@@ -1105,13 +1143,13 @@
         <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="L3" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>40</v>
@@ -1126,7 +1164,7 @@
         <v>33</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>36</v>
@@ -1138,7 +1176,7 @@
         <v>45</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>50</v>
@@ -1168,10 +1206,10 @@
         <v>72</v>
       </c>
       <c r="AE3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF3" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1272,7 +1310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1313,7 +1351,7 @@
         <v>41</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>32</v>
@@ -1334,7 +1372,7 @@
         <v>47</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>38</v>
@@ -1364,46 +1402,46 @@
         <v>38</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C11362729?readertype=staffin"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C1905025?readertype=staffin"/>
-    <hyperlink ref="F2" r:id="rId4" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C2490774?readertype=staffin"/>
-    <hyperlink ref="G2" r:id="rId5" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C1847980?readertype=staffin"/>
-    <hyperlink ref="H2" r:id="rId6"/>
-    <hyperlink ref="I2" r:id="rId7"/>
-    <hyperlink ref="J2" r:id="rId8"/>
-    <hyperlink ref="K2" r:id="rId9"/>
-    <hyperlink ref="L2" r:id="rId10"/>
-    <hyperlink ref="M2" r:id="rId11"/>
-    <hyperlink ref="N2" r:id="rId12"/>
-    <hyperlink ref="O2" r:id="rId13"/>
-    <hyperlink ref="P2" r:id="rId14"/>
-    <hyperlink ref="Q2" r:id="rId15"/>
-    <hyperlink ref="R2" r:id="rId16"/>
-    <hyperlink ref="B2" r:id="rId17" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C4216021?readertype=staffin"/>
-    <hyperlink ref="S2" r:id="rId18"/>
-    <hyperlink ref="T2" r:id="rId19"/>
-    <hyperlink ref="U2" r:id="rId20"/>
-    <hyperlink ref="V2" r:id="rId21"/>
-    <hyperlink ref="W2" r:id="rId22"/>
-    <hyperlink ref="X2" r:id="rId23"/>
-    <hyperlink ref="Y2" r:id="rId24"/>
-    <hyperlink ref="Z2" r:id="rId25"/>
-    <hyperlink ref="AB2" r:id="rId26"/>
-    <hyperlink ref="AC2" r:id="rId27"/>
-    <hyperlink ref="AD2" r:id="rId28"/>
-    <hyperlink ref="AE2" r:id="rId29"/>
-    <hyperlink ref="A2" r:id="rId30"/>
-    <hyperlink ref="AA2" r:id="rId31"/>
-    <hyperlink ref="AF2" r:id="rId32"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C11362729?readertype=staffin" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C1905025?readertype=staffin" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId4" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C2490774?readertype=staffin" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G2" r:id="rId5" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C1847980?readertype=staffin" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I2" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J2" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="K2" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="L2" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="M2" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="N2" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="O2" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="P2" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="Q2" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="R2" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B2" r:id="rId17" display="http://dev.discovery.nationalarchives.gov.uk/details/r/C4216021?readertype=staffin" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="S2" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="V2" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="W2" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="X2" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="Y2" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="Z2" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="AB2" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="AC2" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="AD2" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="AE2" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A2" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="AA2" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="AF2" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="U2" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="T2" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
@@ -1411,7 +1449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
@@ -1423,7 +1461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>